<commit_message>
ajout du code sd + écran
</commit_message>
<xml_diff>
--- a/Freenove_ESP32_WROVER_Board-main/wroversp32freenove_mapping.xlsx
+++ b/Freenove_ESP32_WROVER_Board-main/wroversp32freenove_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\superneiluj\OneDrive\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superneiluj/Desktop/projetelectronique/hornetkiller/Freenove_ESP32_WROVER_Board-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B72440-D93A-48D5-BC7E-E8BA2EF331FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76005A7-9613-C741-B3F4-A948EF9996D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7778349-6BAC-4B27-8BB7-BCD39630D317}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{D7778349-6BAC-4B27-8BB7-BCD39630D317}"/>
   </bookViews>
   <sheets>
     <sheet name="IO Header" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>Utilité</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>CSI Y2</t>
+  </si>
+  <si>
+    <t>CarteSD</t>
+  </si>
+  <si>
+    <t>CarteSD / SD2</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +290,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -564,8 +576,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -593,11 +647,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,31 +659,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -653,52 +713,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,470 +1183,470 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC15C6B-FB90-4E41-922A-A68F7FD5A871}">
   <dimension ref="D2:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D54" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="18" max="18" width="33.7109375" customWidth="1"/>
-    <col min="19" max="19" width="31.85546875" customWidth="1"/>
-    <col min="20" max="20" width="62.28515625" customWidth="1"/>
-    <col min="21" max="21" width="36.5703125" customWidth="1"/>
-    <col min="22" max="22" width="25.7109375" customWidth="1"/>
+    <col min="18" max="18" width="33.6640625" customWidth="1"/>
+    <col min="19" max="19" width="31.83203125" customWidth="1"/>
+    <col min="20" max="20" width="62.33203125" customWidth="1"/>
+    <col min="21" max="21" width="36.5" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
+    <row r="2" spans="4:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="13" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="R14" s="16" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="4:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="23"/>
+    </row>
+    <row r="13" spans="4:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="R14" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="S14" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R15" s="12"/>
-      <c r="S15" s="14"/>
-    </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="R16" s="11">
+    <row r="15" spans="4:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="25"/>
+      <c r="S15" s="27"/>
+    </row>
+    <row r="16" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="R16" s="2">
         <v>1</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R17" s="10">
+    <row r="17" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R17" s="1">
         <v>2</v>
       </c>
-      <c r="S17" s="10" t="s">
+      <c r="S17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R18" s="10">
+    <row r="18" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R18" s="1">
         <v>3</v>
       </c>
-      <c r="S18" s="23" t="s">
+      <c r="S18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="T18" s="18"/>
-    </row>
-    <row r="19" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R19" s="10">
+      <c r="T18" s="28"/>
+    </row>
+    <row r="19" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R19" s="1">
         <v>4</v>
       </c>
-      <c r="S19" s="23" t="s">
+      <c r="S19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T19" s="17"/>
-    </row>
-    <row r="20" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R20" s="10">
+      <c r="T19" s="29"/>
+    </row>
+    <row r="20" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R20" s="1">
         <v>5</v>
       </c>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R21" s="10">
+    <row r="21" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R21" s="1">
         <v>6</v>
       </c>
-      <c r="S21" s="23" t="s">
+      <c r="S21" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R22" s="10">
+    <row r="22" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R22" s="1">
         <v>7</v>
       </c>
-      <c r="S22" s="10" t="s">
+      <c r="S22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R23" s="10">
+    <row r="23" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R23" s="1">
         <v>8</v>
       </c>
-      <c r="S23" s="10" t="s">
+      <c r="S23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R24" s="10">
+    <row r="24" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R24" s="1">
         <v>9</v>
       </c>
-      <c r="S24" s="23" t="s">
+      <c r="S24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R25" s="10">
+    <row r="25" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R25" s="1">
         <v>10</v>
       </c>
-      <c r="S25" s="10" t="s">
+      <c r="S25" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R26" s="10">
+    <row r="26" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R26" s="1">
         <v>11</v>
       </c>
-      <c r="S26" s="10" t="s">
+      <c r="S26" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R27" s="10">
+    <row r="27" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R27" s="1">
         <v>12</v>
       </c>
-      <c r="S27" s="10" t="s">
+      <c r="S27" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R28" s="10">
+    <row r="28" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R28" s="1">
         <v>13</v>
       </c>
-      <c r="S28" s="10" t="s">
+      <c r="S28" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R29" s="10">
+    <row r="29" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R29" s="1">
         <v>14</v>
       </c>
-      <c r="S29" s="10" t="s">
+      <c r="S29" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R30" s="10">
+    <row r="30" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R30" s="1">
         <v>15</v>
       </c>
-      <c r="S30" s="10" t="s">
+      <c r="S30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R31" s="10">
+    <row r="31" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R31" s="1">
         <v>16</v>
       </c>
-      <c r="S31" s="23" t="s">
+      <c r="S31" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R32" s="10">
+    <row r="32" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R32" s="1">
         <v>17</v>
       </c>
-      <c r="S32" s="23" t="s">
+      <c r="S32" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R33" s="10">
+    <row r="33" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R33" s="1">
         <v>18</v>
       </c>
-      <c r="S33" s="23" t="s">
+      <c r="S33" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R34" s="10">
+    <row r="34" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R34" s="1">
         <v>19</v>
       </c>
-      <c r="S34" s="10" t="s">
+      <c r="S34" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R35" s="10">
+    <row r="35" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R35" s="1">
         <v>20</v>
       </c>
-      <c r="S35" s="15" t="s">
+      <c r="S35" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="18:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R39" s="16" t="s">
+    <row r="38" spans="18:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R39" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S39" s="13" t="s">
+      <c r="S39" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="18:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R40" s="12"/>
-      <c r="S40" s="14"/>
-    </row>
-    <row r="41" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R41" s="11">
+    <row r="40" spans="18:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="25"/>
+      <c r="S40" s="27"/>
+    </row>
+    <row r="41" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R41" s="2">
         <v>1</v>
       </c>
-      <c r="S41" s="10" t="s">
+      <c r="S41" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R42" s="10">
+    <row r="42" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R42" s="1">
         <v>2</v>
       </c>
-      <c r="S42" s="23" t="s">
+      <c r="S42" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="18:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R43" s="10">
+    <row r="43" spans="18:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R43" s="1">
         <v>3</v>
       </c>
-      <c r="S43" s="42" t="s">
+      <c r="S43" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R44" s="41">
+    <row r="44" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R44" s="7">
         <v>4</v>
       </c>
-      <c r="S44" s="43" t="s">
+      <c r="S44" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T44" s="38" t="s">
+      <c r="T44" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R45" s="41">
+    <row r="45" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R45" s="7">
         <v>5</v>
       </c>
-      <c r="S45" s="44" t="s">
+      <c r="S45" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="T45" s="39"/>
-    </row>
-    <row r="46" spans="18:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R46" s="41">
+      <c r="T45" s="13"/>
+    </row>
+    <row r="46" spans="18:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R46" s="7">
         <v>6</v>
       </c>
-      <c r="S46" s="45" t="s">
+      <c r="S46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="T46" s="40"/>
-    </row>
-    <row r="47" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R47" s="10">
+      <c r="T46" s="14"/>
+    </row>
+    <row r="47" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R47" s="1">
         <v>7</v>
       </c>
-      <c r="S47" s="11" t="s">
+      <c r="S47" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R48" s="10">
+    <row r="48" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R48" s="1">
         <v>8</v>
       </c>
-      <c r="S48" s="23" t="s">
+      <c r="S48" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R49" s="10">
+    <row r="49" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R49" s="1">
         <v>9</v>
       </c>
-      <c r="S49" s="23" t="s">
+      <c r="S49" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R50" s="10">
+    <row r="50" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R50" s="1">
         <v>10</v>
       </c>
-      <c r="S50" s="23" t="s">
+      <c r="S50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R51" s="10">
+    <row r="51" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R51" s="1">
         <v>11</v>
       </c>
-      <c r="S51" s="10" t="s">
+      <c r="S51" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R52" s="10">
+    <row r="52" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R52" s="1">
         <v>12</v>
       </c>
-      <c r="S52" s="10" t="s">
+      <c r="S52" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R53" s="10">
+    <row r="53" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R53" s="1">
         <v>13</v>
       </c>
-      <c r="S53" s="23" t="s">
+      <c r="S53" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R54" s="10">
+    <row r="54" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R54" s="1">
         <v>14</v>
       </c>
-      <c r="S54" s="10" t="s">
+      <c r="S54" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R55" s="10">
+    <row r="55" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R55" s="1">
         <v>15</v>
       </c>
-      <c r="S55" s="10" t="s">
+      <c r="S55" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R56" s="10">
+    <row r="56" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R56" s="1">
         <v>16</v>
       </c>
-      <c r="S56" s="10" t="s">
+      <c r="S56" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R57" s="10">
+    <row r="57" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R57" s="1">
         <v>17</v>
       </c>
-      <c r="S57" s="23" t="s">
+      <c r="S57" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R58" s="10">
+    <row r="58" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R58" s="1">
         <v>18</v>
       </c>
-      <c r="S58" s="23" t="s">
+      <c r="S58" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R59" s="10">
+    <row r="59" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R59" s="1">
         <v>19</v>
       </c>
-      <c r="S59" s="10" t="s">
+      <c r="S59" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R60" s="10">
+    <row r="60" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R60" s="1">
         <v>20</v>
       </c>
-      <c r="S60" s="15" t="s">
+      <c r="S60" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1649,488 +1670,488 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B22FE44-2213-4176-BB0D-28CE9A95AF90}">
   <dimension ref="D3:W57"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="F26" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="19" max="19" width="24.5703125" customWidth="1"/>
-    <col min="20" max="20" width="43.85546875" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" customWidth="1"/>
-    <col min="23" max="23" width="41.7109375" customWidth="1"/>
+    <col min="19" max="19" width="24.5" customWidth="1"/>
+    <col min="20" max="20" width="43.83203125" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" customWidth="1"/>
+    <col min="23" max="23" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
+    <row r="3" spans="4:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="4:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="13" spans="4:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="4:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S14" s="19" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="4:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="23"/>
+    </row>
+    <row r="13" spans="4:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:23" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="T14" s="20" t="s">
+      <c r="T14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="V14" s="24" t="s">
+      <c r="V14" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="W14" s="25"/>
-    </row>
-    <row r="15" spans="4:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S15" s="21"/>
-      <c r="T15" s="22"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="27"/>
-    </row>
-    <row r="16" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="S16" s="11">
+      <c r="W14" s="41"/>
+    </row>
+    <row r="15" spans="4:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="37"/>
+      <c r="T15" s="39"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="43"/>
+    </row>
+    <row r="16" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="S16" s="2">
         <v>1</v>
       </c>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V16" s="26"/>
-      <c r="W16" s="27"/>
-    </row>
-    <row r="17" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S17" s="10">
+      <c r="V16" s="42"/>
+      <c r="W16" s="43"/>
+    </row>
+    <row r="17" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S17" s="1">
         <v>2</v>
       </c>
-      <c r="T17" s="10" t="s">
+      <c r="T17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V17" s="26"/>
-      <c r="W17" s="27"/>
-    </row>
-    <row r="18" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S18" s="10">
+      <c r="V17" s="42"/>
+      <c r="W17" s="43"/>
+    </row>
+    <row r="18" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S18" s="1">
         <v>3</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V18" s="26"/>
-      <c r="W18" s="27"/>
-    </row>
-    <row r="19" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S19" s="10">
+      <c r="V18" s="42"/>
+      <c r="W18" s="43"/>
+    </row>
+    <row r="19" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S19" s="1">
         <v>4</v>
       </c>
-      <c r="T19" s="10" t="s">
+      <c r="T19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V19" s="26"/>
-      <c r="W19" s="27"/>
-    </row>
-    <row r="20" spans="19:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S20" s="10">
+      <c r="V19" s="42"/>
+      <c r="W19" s="43"/>
+    </row>
+    <row r="20" spans="19:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S20" s="1">
         <v>5</v>
       </c>
-      <c r="T20" s="10" t="s">
+      <c r="T20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V20" s="28"/>
-      <c r="W20" s="29"/>
-    </row>
-    <row r="21" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S21" s="10">
+      <c r="V20" s="44"/>
+      <c r="W20" s="45"/>
+    </row>
+    <row r="21" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S21" s="1">
         <v>6</v>
       </c>
-      <c r="T21" s="10" t="s">
+      <c r="T21" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="19:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S22" s="10">
+    <row r="22" spans="19:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S22" s="1">
         <v>7</v>
       </c>
-      <c r="T22" s="10" t="s">
+      <c r="T22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S23" s="10">
+    <row r="23" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S23" s="1">
         <v>8</v>
       </c>
-      <c r="T23" s="10" t="s">
+      <c r="T23" s="48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="19:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="1">
+        <v>9</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S25" s="1">
+        <v>10</v>
+      </c>
+      <c r="T25" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="V25" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="W25" s="31"/>
+    </row>
+    <row r="26" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S26" s="1">
+        <v>11</v>
+      </c>
+      <c r="T26" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="V26" s="32"/>
+      <c r="W26" s="33"/>
+    </row>
+    <row r="27" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S27" s="1">
+        <v>12</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V27" s="32"/>
+      <c r="W27" s="33"/>
+    </row>
+    <row r="28" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S28" s="1">
+        <v>13</v>
+      </c>
+      <c r="T28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="V28" s="32"/>
+      <c r="W28" s="33"/>
+    </row>
+    <row r="29" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S29" s="1">
+        <v>14</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V29" s="32"/>
+      <c r="W29" s="33"/>
+    </row>
+    <row r="30" spans="19:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="19:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S24" s="10">
-        <v>9</v>
-      </c>
-      <c r="T24" s="30" t="s">
+      <c r="T30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V30" s="34"/>
+      <c r="W30" s="35"/>
+    </row>
+    <row r="31" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S31" s="1">
+        <v>16</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S32" s="1">
+        <v>17</v>
+      </c>
+      <c r="T32" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S33" s="1">
+        <v>18</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S34" s="1">
+        <v>19</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="19:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S37" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="T37" s="38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="19:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S38" s="37"/>
+      <c r="T38" s="39"/>
+    </row>
+    <row r="39" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S39" s="2">
+        <v>20</v>
+      </c>
+      <c r="T39" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S40" s="2">
+        <v>21</v>
+      </c>
+      <c r="T40" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S41" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S25" s="10">
-        <v>10</v>
-      </c>
-      <c r="T25" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="V25" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="W25" s="33"/>
-    </row>
-    <row r="26" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S26" s="10">
-        <v>11</v>
-      </c>
-      <c r="T26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="V26" s="34"/>
-      <c r="W26" s="35"/>
-    </row>
-    <row r="27" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S27" s="10">
-        <v>12</v>
-      </c>
-      <c r="T27" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="V27" s="34"/>
-      <c r="W27" s="35"/>
-    </row>
-    <row r="28" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S28" s="10">
-        <v>13</v>
-      </c>
-      <c r="T28" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="V28" s="34"/>
-      <c r="W28" s="35"/>
-    </row>
-    <row r="29" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S29" s="10">
-        <v>14</v>
-      </c>
-      <c r="T29" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V29" s="34"/>
-      <c r="W29" s="35"/>
-    </row>
-    <row r="30" spans="19:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S30" s="10">
-        <v>15</v>
-      </c>
-      <c r="T30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V30" s="36"/>
-      <c r="W30" s="37"/>
-    </row>
-    <row r="31" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S31" s="10">
-        <v>16</v>
-      </c>
-      <c r="T31" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="19:23" x14ac:dyDescent="0.25">
-      <c r="S32" s="10">
-        <v>17</v>
-      </c>
-      <c r="T32" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S33" s="10">
-        <v>18</v>
-      </c>
-      <c r="T33" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S34" s="10">
-        <v>19</v>
-      </c>
-      <c r="T34" s="23" t="s">
+      <c r="T41" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S42" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="19:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S37" s="19" t="s">
+      <c r="T42" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S43" s="2">
         <v>24</v>
       </c>
-      <c r="T37" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="19:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S38" s="21"/>
-      <c r="T38" s="22"/>
-    </row>
-    <row r="39" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S39" s="11">
-        <v>20</v>
-      </c>
-      <c r="T39" s="23" t="s">
+      <c r="T43" s="48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S44" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S40" s="11">
-        <v>21</v>
-      </c>
-      <c r="T40" s="23" t="s">
+      <c r="T44" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S45" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S41" s="11">
-        <v>22</v>
-      </c>
-      <c r="T41" s="23" t="s">
+      <c r="T45" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S46" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S42" s="11">
-        <v>23</v>
-      </c>
-      <c r="T42" s="10" t="s">
+      <c r="T46" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S47" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S43" s="11">
-        <v>24</v>
-      </c>
-      <c r="T43" s="10" t="s">
+      <c r="T47" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S48" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S44" s="11">
-        <v>25</v>
-      </c>
-      <c r="T44" s="10" t="s">
+      <c r="T48" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S49" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S45" s="11">
-        <v>26</v>
-      </c>
-      <c r="T45" s="10" t="s">
+      <c r="T49" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S50" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S46" s="11">
-        <v>27</v>
-      </c>
-      <c r="T46" s="23" t="s">
+      <c r="T50" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S51" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S47" s="11">
-        <v>28</v>
-      </c>
-      <c r="T47" s="31" t="s">
+      <c r="T51" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S48" s="11">
-        <v>29</v>
-      </c>
-      <c r="T48" s="10" t="s">
+    <row r="52" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S52" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S49" s="11">
-        <v>30</v>
-      </c>
-      <c r="T49" s="10" t="s">
+      <c r="T52" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S53" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S50" s="11">
-        <v>31</v>
-      </c>
-      <c r="T50" s="15" t="s">
+      <c r="T53" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S54" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S51" s="11">
-        <v>32</v>
-      </c>
-      <c r="T51" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S52" s="11">
-        <v>33</v>
-      </c>
-      <c r="T52" s="10" t="s">
+      <c r="T54" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S55" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S53" s="11">
-        <v>34</v>
-      </c>
-      <c r="T53" s="10" t="s">
+      <c r="T55" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S56" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="54" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S54" s="11">
-        <v>35</v>
-      </c>
-      <c r="T54" s="10" t="s">
+      <c r="T56" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S57" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="55" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S55" s="11">
-        <v>36</v>
-      </c>
-      <c r="T55" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S56" s="11">
-        <v>37</v>
-      </c>
-      <c r="T56" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="19:20" x14ac:dyDescent="0.25">
-      <c r="S57" s="11">
-        <v>38</v>
-      </c>
-      <c r="T57" s="10" t="s">
+      <c r="T57" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="S37:S38"/>
+    <mergeCell ref="T37:T38"/>
     <mergeCell ref="V25:W30"/>
     <mergeCell ref="D4:O10"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="T14:T15"/>
     <mergeCell ref="V14:W20"/>
-    <mergeCell ref="S37:S38"/>
-    <mergeCell ref="T37:T38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>